<commit_message>
finish label intact...will organize tmr
</commit_message>
<xml_diff>
--- a/Book2.xlsx
+++ b/Book2.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent.Zhong\Documents\GitHub\Label_Star_Info\File Uploader\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent.Zhong\Documents\GitHub\Label_Star\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6466115-8E4B-420C-B091-77F1982376A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50FF2F11-FDE8-48C0-85E3-FB3ECDE9538E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8A430301-C3A3-451D-9275-EE1F2FAE0B57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet12" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet12!$A$1:$O$501</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -5092,7 +5095,7 @@
   <dimension ref="A1:O501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:O1"/>
+      <selection activeCell="F13" sqref="A1:O501"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28645,6 +28648,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:O501" xr:uid="{F5BDC2B3-F5E5-4DE2-9544-370C45622D3F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>